<commit_message>
Updated source file for Land Conflict Watch
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/LCW-LCI/LCW-LCI.xlsx
+++ b/Simple_XLS_Importer/data/LCW-LCI/LCW-LCI.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\vm\debian8.2-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\@landportal.info\Land Book\LCW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="3" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000"/>
@@ -20,15 +20,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="17">
   <si>
     <t>org_acronym</t>
   </si>
@@ -121,10 +118,59 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -133,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -143,11 +189,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,20 +477,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182:B241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.296875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="10.796875" style="6"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -478,10 +520,10 @@
       <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7">
-        <v>1921</v>
-      </c>
-      <c r="D3" s="8">
+      <c r="C3" s="11">
+        <v>1916</v>
+      </c>
+      <c r="D3" s="12">
         <v>1</v>
       </c>
     </row>
@@ -492,10 +534,10 @@
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7">
-        <v>1938</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="C4" s="11">
+        <v>1921</v>
+      </c>
+      <c r="D4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -506,10 +548,10 @@
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7">
-        <v>1941</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="C5" s="11">
+        <v>1938</v>
+      </c>
+      <c r="D5" s="12">
         <v>1</v>
       </c>
     </row>
@@ -520,11 +562,11 @@
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7">
-        <v>1950</v>
-      </c>
-      <c r="D6" s="8">
-        <v>2</v>
+      <c r="C6" s="11">
+        <v>1941</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -534,10 +576,10 @@
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7">
-        <v>1952</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="C7" s="11">
+        <v>1946</v>
+      </c>
+      <c r="D7" s="12">
         <v>1</v>
       </c>
     </row>
@@ -548,11 +590,11 @@
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7">
-        <v>1955</v>
-      </c>
-      <c r="D8" s="8">
-        <v>1</v>
+      <c r="C8" s="11">
+        <v>1950</v>
+      </c>
+      <c r="D8" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -562,11 +604,11 @@
       <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7">
-        <v>1956</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
+      <c r="C9" s="11">
+        <v>1952</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -576,11 +618,11 @@
       <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7">
-        <v>1962</v>
-      </c>
-      <c r="D10" s="8">
-        <v>2</v>
+      <c r="C10" s="11">
+        <v>1955</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -590,10 +632,10 @@
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7">
-        <v>1967</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="C11" s="11">
+        <v>1956</v>
+      </c>
+      <c r="D11" s="12">
         <v>1</v>
       </c>
     </row>
@@ -604,11 +646,11 @@
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7">
-        <v>1970</v>
-      </c>
-      <c r="D12" s="8">
-        <v>4</v>
+      <c r="C12" s="11">
+        <v>1959</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -618,10 +660,10 @@
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7">
-        <v>1972</v>
-      </c>
-      <c r="D13" s="8">
+      <c r="C13" s="11">
+        <v>1960</v>
+      </c>
+      <c r="D13" s="12">
         <v>2</v>
       </c>
     </row>
@@ -632,11 +674,11 @@
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7">
-        <v>1973</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1</v>
+      <c r="C14" s="11">
+        <v>1962</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -646,11 +688,11 @@
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="7">
-        <v>1974</v>
-      </c>
-      <c r="D15" s="8">
-        <v>2</v>
+      <c r="C15" s="11">
+        <v>1967</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -660,11 +702,11 @@
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="7">
-        <v>1975</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
+      <c r="C16" s="11">
+        <v>1970</v>
+      </c>
+      <c r="D16" s="12">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -674,11 +716,11 @@
       <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7">
-        <v>1978</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
+      <c r="C17" s="11">
+        <v>1972</v>
+      </c>
+      <c r="D17" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -688,10 +730,10 @@
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="7">
-        <v>1979</v>
-      </c>
-      <c r="D18" s="8">
+      <c r="C18" s="11">
+        <v>1973</v>
+      </c>
+      <c r="D18" s="12">
         <v>2</v>
       </c>
     </row>
@@ -702,11 +744,11 @@
       <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="7">
-        <v>1980</v>
-      </c>
-      <c r="D19" s="8">
-        <v>4</v>
+      <c r="C19" s="11">
+        <v>1974</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -716,10 +758,10 @@
       <c r="B20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="7">
-        <v>1981</v>
-      </c>
-      <c r="D20" s="8">
+      <c r="C20" s="11">
+        <v>1975</v>
+      </c>
+      <c r="D20" s="12">
         <v>1</v>
       </c>
     </row>
@@ -730,11 +772,11 @@
       <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="7">
-        <v>1982</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1</v>
+      <c r="C21" s="11">
+        <v>1976</v>
+      </c>
+      <c r="D21" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -744,11 +786,11 @@
       <c r="B22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="7">
-        <v>1983</v>
-      </c>
-      <c r="D22" s="8">
-        <v>1</v>
+      <c r="C22" s="11">
+        <v>1978</v>
+      </c>
+      <c r="D22" s="12">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -758,11 +800,11 @@
       <c r="B23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="7">
-        <v>1984</v>
-      </c>
-      <c r="D23" s="8">
-        <v>1</v>
+      <c r="C23" s="11">
+        <v>1979</v>
+      </c>
+      <c r="D23" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -772,11 +814,11 @@
       <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="7">
-        <v>1985</v>
-      </c>
-      <c r="D24" s="8">
-        <v>1</v>
+      <c r="C24" s="11">
+        <v>1980</v>
+      </c>
+      <c r="D24" s="12">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -786,10 +828,10 @@
       <c r="B25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="7">
-        <v>1987</v>
-      </c>
-      <c r="D25" s="8">
+      <c r="C25" s="11">
+        <v>1981</v>
+      </c>
+      <c r="D25" s="12">
         <v>1</v>
       </c>
     </row>
@@ -800,10 +842,10 @@
       <c r="B26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="7">
-        <v>1988</v>
-      </c>
-      <c r="D26" s="8">
+      <c r="C26" s="11">
+        <v>1982</v>
+      </c>
+      <c r="D26" s="12">
         <v>1</v>
       </c>
     </row>
@@ -814,11 +856,11 @@
       <c r="B27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="7">
-        <v>1989</v>
-      </c>
-      <c r="D27" s="8">
-        <v>2</v>
+      <c r="C27" s="11">
+        <v>1983</v>
+      </c>
+      <c r="D27" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -828,10 +870,10 @@
       <c r="B28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="7">
-        <v>1990</v>
-      </c>
-      <c r="D28" s="8">
+      <c r="C28" s="11">
+        <v>1984</v>
+      </c>
+      <c r="D28" s="12">
         <v>1</v>
       </c>
     </row>
@@ -842,11 +884,11 @@
       <c r="B29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="7">
-        <v>1991</v>
-      </c>
-      <c r="D29" s="8">
-        <v>1</v>
+      <c r="C29" s="11">
+        <v>1985</v>
+      </c>
+      <c r="D29" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -856,10 +898,10 @@
       <c r="B30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="7">
-        <v>1992</v>
-      </c>
-      <c r="D30" s="8">
+      <c r="C30" s="11">
+        <v>1987</v>
+      </c>
+      <c r="D30" s="12">
         <v>4</v>
       </c>
     </row>
@@ -870,11 +912,11 @@
       <c r="B31" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="7">
-        <v>1994</v>
-      </c>
-      <c r="D31" s="8">
-        <v>5</v>
+      <c r="C31" s="11">
+        <v>1988</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -884,11 +926,11 @@
       <c r="B32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="7">
-        <v>1995</v>
-      </c>
-      <c r="D32" s="8">
-        <v>1</v>
+      <c r="C32" s="11">
+        <v>1989</v>
+      </c>
+      <c r="D32" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -898,10 +940,10 @@
       <c r="B33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="7">
-        <v>1996</v>
-      </c>
-      <c r="D33" s="8">
+      <c r="C33" s="11">
+        <v>1990</v>
+      </c>
+      <c r="D33" s="12">
         <v>2</v>
       </c>
     </row>
@@ -912,11 +954,11 @@
       <c r="B34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="7">
-        <v>1997</v>
-      </c>
-      <c r="D34" s="8">
-        <v>1</v>
+      <c r="C34" s="11">
+        <v>1991</v>
+      </c>
+      <c r="D34" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -926,11 +968,11 @@
       <c r="B35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="7">
-        <v>1998</v>
-      </c>
-      <c r="D35" s="8">
-        <v>2</v>
+      <c r="C35" s="11">
+        <v>1992</v>
+      </c>
+      <c r="D35" s="12">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -940,11 +982,11 @@
       <c r="B36" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D36" s="8">
-        <v>4</v>
+      <c r="C36" s="11">
+        <v>1993</v>
+      </c>
+      <c r="D36" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -954,11 +996,11 @@
       <c r="B37" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="7">
-        <v>2001</v>
-      </c>
-      <c r="D37" s="8">
-        <v>4</v>
+      <c r="C37" s="11">
+        <v>1994</v>
+      </c>
+      <c r="D37" s="12">
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -968,10 +1010,10 @@
       <c r="B38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D38" s="8">
+      <c r="C38" s="11">
+        <v>1995</v>
+      </c>
+      <c r="D38" s="12">
         <v>3</v>
       </c>
     </row>
@@ -982,11 +1024,11 @@
       <c r="B39" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D39" s="8">
-        <v>4</v>
+      <c r="C39" s="11">
+        <v>1996</v>
+      </c>
+      <c r="D39" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -996,11 +1038,11 @@
       <c r="B40" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D40" s="8">
-        <v>2</v>
+      <c r="C40" s="11">
+        <v>1997</v>
+      </c>
+      <c r="D40" s="12">
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1010,11 +1052,11 @@
       <c r="B41" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D41" s="8">
-        <v>9</v>
+      <c r="C41" s="11">
+        <v>1998</v>
+      </c>
+      <c r="D41" s="12">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1024,11 +1066,11 @@
       <c r="B42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="7">
-        <v>2006</v>
-      </c>
-      <c r="D42" s="8">
-        <v>8</v>
+      <c r="C42" s="11">
+        <v>1999</v>
+      </c>
+      <c r="D42" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1038,11 +1080,11 @@
       <c r="B43" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="7">
-        <v>2007</v>
-      </c>
-      <c r="D43" s="8">
-        <v>13</v>
+      <c r="C43" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D43" s="12">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1052,11 +1094,11 @@
       <c r="B44" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D44" s="8">
-        <v>15</v>
+      <c r="C44" s="11">
+        <v>2001</v>
+      </c>
+      <c r="D44" s="12">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1066,11 +1108,11 @@
       <c r="B45" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D45" s="8">
-        <v>17</v>
+      <c r="C45" s="11">
+        <v>2002</v>
+      </c>
+      <c r="D45" s="12">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1080,11 +1122,11 @@
       <c r="B46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="7">
-        <v>2010</v>
-      </c>
-      <c r="D46" s="8">
-        <v>12</v>
+      <c r="C46" s="11">
+        <v>2003</v>
+      </c>
+      <c r="D46" s="12">
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1094,11 +1136,11 @@
       <c r="B47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="7">
-        <v>2011</v>
-      </c>
-      <c r="D47" s="8">
-        <v>14</v>
+      <c r="C47" s="11">
+        <v>2004</v>
+      </c>
+      <c r="D47" s="12">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1108,11 +1150,11 @@
       <c r="B48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="7">
-        <v>2012</v>
-      </c>
-      <c r="D48" s="8">
-        <v>16</v>
+      <c r="C48" s="11">
+        <v>2005</v>
+      </c>
+      <c r="D48" s="12">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1122,11 +1164,11 @@
       <c r="B49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="7">
-        <v>2013</v>
-      </c>
-      <c r="D49" s="8">
-        <v>16</v>
+      <c r="C49" s="11">
+        <v>2006</v>
+      </c>
+      <c r="D49" s="12">
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1136,10 +1178,10 @@
       <c r="B50" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="7">
-        <v>2014</v>
-      </c>
-      <c r="D50" s="8">
+      <c r="C50" s="11">
+        <v>2007</v>
+      </c>
+      <c r="D50" s="12">
         <v>23</v>
       </c>
     </row>
@@ -1150,11 +1192,11 @@
       <c r="B51" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="7">
-        <v>2015</v>
-      </c>
-      <c r="D51" s="8">
-        <v>40</v>
+      <c r="C51" s="11">
+        <v>2008</v>
+      </c>
+      <c r="D51" s="12">
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1164,11 +1206,11 @@
       <c r="B52" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="7">
-        <v>2016</v>
-      </c>
-      <c r="D52" s="8">
-        <v>36</v>
+      <c r="C52" s="11">
+        <v>2009</v>
+      </c>
+      <c r="D52" s="12">
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1178,123 +1220,123 @@
       <c r="B53" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D53" s="8">
-        <v>2</v>
+      <c r="C53" s="11">
+        <v>2010</v>
+      </c>
+      <c r="D53" s="12">
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="7">
-        <v>1912</v>
-      </c>
-      <c r="D54" s="8">
-        <v>24</v>
+      <c r="C54" s="11">
+        <v>2011</v>
+      </c>
+      <c r="D54" s="12">
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="7">
-        <v>1921</v>
-      </c>
-      <c r="D55" s="8">
-        <v>576</v>
+      <c r="C55" s="11">
+        <v>2012</v>
+      </c>
+      <c r="D55" s="12">
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="7">
-        <v>1938</v>
-      </c>
-      <c r="D56" s="8">
-        <v>192</v>
+      <c r="C56" s="11">
+        <v>2013</v>
+      </c>
+      <c r="D56" s="12">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="7">
-        <v>1941</v>
-      </c>
-      <c r="D57" s="8">
-        <v>3840</v>
+      <c r="C57" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D57" s="12">
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="7">
-        <v>1950</v>
-      </c>
-      <c r="D58" s="8">
-        <v>19461</v>
+      <c r="C58" s="11">
+        <v>2015</v>
+      </c>
+      <c r="D58" s="12">
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="7">
-        <v>1952</v>
-      </c>
-      <c r="D59" s="8">
-        <v>763.19999999999993</v>
+      <c r="C59" s="11">
+        <v>2016</v>
+      </c>
+      <c r="D59" s="12">
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="7">
-        <v>1955</v>
-      </c>
-      <c r="D60" s="8">
-        <v>720</v>
+      <c r="C60" s="11">
+        <v>2017</v>
+      </c>
+      <c r="D60" s="12">
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="7">
-        <v>1956</v>
-      </c>
-      <c r="D61" s="8">
-        <v>47582.400000000001</v>
+      <c r="C61" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D61" s="12">
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1305,10 +1347,10 @@
         <v>12</v>
       </c>
       <c r="C62" s="7">
-        <v>1962</v>
-      </c>
-      <c r="D62" s="8">
-        <v>3115.2</v>
+        <v>1912</v>
+      </c>
+      <c r="D62" s="9">
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1318,11 +1360,11 @@
       <c r="B63" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="7">
-        <v>1967</v>
-      </c>
-      <c r="D63" s="8">
-        <v>4800</v>
+      <c r="C63" s="11">
+        <v>1916</v>
+      </c>
+      <c r="D63" s="13">
+        <v>114465.59999999999</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1332,11 +1374,11 @@
       <c r="B64" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="7">
-        <v>1970</v>
-      </c>
-      <c r="D64" s="8">
-        <v>25630.799999999999</v>
+      <c r="C64" s="11">
+        <v>1921</v>
+      </c>
+      <c r="D64" s="13">
+        <v>576</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1346,11 +1388,11 @@
       <c r="B65" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="7">
-        <v>1972</v>
-      </c>
-      <c r="D65" s="8">
-        <v>288</v>
+      <c r="C65" s="11">
+        <v>1938</v>
+      </c>
+      <c r="D65" s="13">
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1360,11 +1402,11 @@
       <c r="B66" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="7">
-        <v>1973</v>
-      </c>
-      <c r="D66" s="8">
-        <v>400</v>
+      <c r="C66" s="11">
+        <v>1941</v>
+      </c>
+      <c r="D66" s="13">
+        <v>3840</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1374,12 +1416,10 @@
       <c r="B67" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="7">
-        <v>1974</v>
-      </c>
-      <c r="D67" s="8">
-        <v>758.4</v>
-      </c>
+      <c r="C67" s="11">
+        <v>1946</v>
+      </c>
+      <c r="D67" s="13"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
@@ -1388,11 +1428,11 @@
       <c r="B68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="7">
-        <v>1975</v>
-      </c>
-      <c r="D68" s="8">
-        <v>9500</v>
+      <c r="C68" s="11">
+        <v>1950</v>
+      </c>
+      <c r="D68" s="13">
+        <v>19461</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1402,11 +1442,11 @@
       <c r="B69" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="7">
-        <v>1978</v>
-      </c>
-      <c r="D69" s="8">
-        <v>2000</v>
+      <c r="C69" s="11">
+        <v>1952</v>
+      </c>
+      <c r="D69" s="13">
+        <v>10763.2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1416,11 +1456,11 @@
       <c r="B70" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C70" s="7">
-        <v>1979</v>
-      </c>
-      <c r="D70" s="8">
-        <v>41102.400000000001</v>
+      <c r="C70" s="11">
+        <v>1955</v>
+      </c>
+      <c r="D70" s="13">
+        <v>720</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1430,11 +1470,11 @@
       <c r="B71" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="7">
-        <v>1980</v>
-      </c>
-      <c r="D71" s="8">
-        <v>12500</v>
+      <c r="C71" s="11">
+        <v>1956</v>
+      </c>
+      <c r="D71" s="13">
+        <v>47582.400000000001</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1444,11 +1484,11 @@
       <c r="B72" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="7">
-        <v>1981</v>
-      </c>
-      <c r="D72" s="8">
-        <v>3840</v>
+      <c r="C72" s="11">
+        <v>1959</v>
+      </c>
+      <c r="D72" s="13">
+        <v>19651.2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,11 +1498,11 @@
       <c r="B73" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="7">
-        <v>1982</v>
-      </c>
-      <c r="D73" s="8">
-        <v>79000</v>
+      <c r="C73" s="11">
+        <v>1960</v>
+      </c>
+      <c r="D73" s="13">
+        <v>31000</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1472,11 +1512,11 @@
       <c r="B74" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C74" s="7">
-        <v>1983</v>
-      </c>
-      <c r="D74" s="8">
-        <v>500</v>
+      <c r="C74" s="11">
+        <v>1962</v>
+      </c>
+      <c r="D74" s="13">
+        <v>3115.2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,11 +1526,11 @@
       <c r="B75" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="7">
-        <v>1984</v>
-      </c>
-      <c r="D75" s="8">
-        <v>960</v>
+      <c r="C75" s="11">
+        <v>1967</v>
+      </c>
+      <c r="D75" s="13">
+        <v>4800</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,11 +1540,11 @@
       <c r="B76" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C76" s="7">
-        <v>1985</v>
-      </c>
-      <c r="D76" s="8">
-        <v>8153</v>
+      <c r="C76" s="11">
+        <v>1970</v>
+      </c>
+      <c r="D76" s="13">
+        <v>25630.799999999999</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1514,11 +1554,11 @@
       <c r="B77" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="7">
-        <v>1987</v>
-      </c>
-      <c r="D77" s="8">
-        <v>76000</v>
+      <c r="C77" s="11">
+        <v>1972</v>
+      </c>
+      <c r="D77" s="13">
+        <v>3456</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1528,11 +1568,11 @@
       <c r="B78" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="7">
-        <v>1988</v>
-      </c>
-      <c r="D78" s="8">
-        <v>20798.399999999998</v>
+      <c r="C78" s="11">
+        <v>1973</v>
+      </c>
+      <c r="D78" s="13">
+        <v>7844.7999999999993</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1542,11 +1582,11 @@
       <c r="B79" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C79" s="7">
-        <v>1989</v>
-      </c>
-      <c r="D79" s="8">
-        <v>13000</v>
+      <c r="C79" s="11">
+        <v>1974</v>
+      </c>
+      <c r="D79" s="13">
+        <v>758.4</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1556,11 +1596,11 @@
       <c r="B80" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="7">
-        <v>1990</v>
-      </c>
-      <c r="D80" s="8">
-        <v>0</v>
+      <c r="C80" s="11">
+        <v>1975</v>
+      </c>
+      <c r="D80" s="13">
+        <v>9500</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1570,11 +1610,11 @@
       <c r="B81" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="7">
-        <v>1991</v>
-      </c>
-      <c r="D81" s="8">
-        <v>1000</v>
+      <c r="C81" s="11">
+        <v>1976</v>
+      </c>
+      <c r="D81" s="13">
+        <v>14400</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1584,11 +1624,11 @@
       <c r="B82" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C82" s="7">
-        <v>1992</v>
-      </c>
-      <c r="D82" s="8">
-        <v>18748.8</v>
+      <c r="C82" s="11">
+        <v>1978</v>
+      </c>
+      <c r="D82" s="13">
+        <v>48352</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1598,11 +1638,11 @@
       <c r="B83" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C83" s="7">
-        <v>1994</v>
-      </c>
-      <c r="D83" s="8">
-        <v>23293.599999999999</v>
+      <c r="C83" s="11">
+        <v>1979</v>
+      </c>
+      <c r="D83" s="13">
+        <v>41102.400000000001</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1612,11 +1652,11 @@
       <c r="B84" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="7">
-        <v>1995</v>
-      </c>
-      <c r="D84" s="8">
-        <v>43200</v>
+      <c r="C84" s="11">
+        <v>1980</v>
+      </c>
+      <c r="D84" s="13">
+        <v>26007.200000000001</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1626,11 +1666,11 @@
       <c r="B85" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C85" s="7">
-        <v>1996</v>
-      </c>
-      <c r="D85" s="8">
-        <v>6652.8</v>
+      <c r="C85" s="11">
+        <v>1981</v>
+      </c>
+      <c r="D85" s="13">
+        <v>3840</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1640,11 +1680,11 @@
       <c r="B86" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C86" s="7">
-        <v>1997</v>
-      </c>
-      <c r="D86" s="8">
-        <v>2920</v>
+      <c r="C86" s="11">
+        <v>1982</v>
+      </c>
+      <c r="D86" s="13">
+        <v>79000</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1654,11 +1694,11 @@
       <c r="B87" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C87" s="7">
-        <v>1998</v>
-      </c>
-      <c r="D87" s="8">
-        <v>2140</v>
+      <c r="C87" s="11">
+        <v>1983</v>
+      </c>
+      <c r="D87" s="13">
+        <v>100980</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1668,11 +1708,11 @@
       <c r="B88" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C88" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D88" s="8">
-        <v>16768</v>
+      <c r="C88" s="11">
+        <v>1984</v>
+      </c>
+      <c r="D88" s="13">
+        <v>960</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -1682,11 +1722,11 @@
       <c r="B89" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="7">
-        <v>2001</v>
-      </c>
-      <c r="D89" s="8">
-        <v>50433.599999999999</v>
+      <c r="C89" s="11">
+        <v>1985</v>
+      </c>
+      <c r="D89" s="13">
+        <v>38153</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1696,11 +1736,11 @@
       <c r="B90" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D90" s="8">
-        <v>537038.4</v>
+      <c r="C90" s="11">
+        <v>1987</v>
+      </c>
+      <c r="D90" s="13">
+        <v>76720</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -1710,11 +1750,11 @@
       <c r="B91" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C91" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D91" s="8">
-        <v>94400</v>
+      <c r="C91" s="11">
+        <v>1988</v>
+      </c>
+      <c r="D91" s="13">
+        <v>20798.399999999998</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1724,11 +1764,11 @@
       <c r="B92" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D92" s="8">
-        <v>7360</v>
+      <c r="C92" s="11">
+        <v>1989</v>
+      </c>
+      <c r="D92" s="13">
+        <v>13590.4</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -1738,11 +1778,11 @@
       <c r="B93" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D93" s="8">
-        <v>52665.8</v>
+      <c r="C93" s="11">
+        <v>1990</v>
+      </c>
+      <c r="D93" s="13">
+        <v>50000</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,11 +1792,11 @@
       <c r="B94" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="7">
-        <v>2006</v>
-      </c>
-      <c r="D94" s="8">
-        <v>75552.800000000003</v>
+      <c r="C94" s="11">
+        <v>1991</v>
+      </c>
+      <c r="D94" s="13">
+        <v>11440</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -1766,11 +1806,11 @@
       <c r="B95" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C95" s="7">
-        <v>2007</v>
-      </c>
-      <c r="D95" s="8">
-        <v>73043.8</v>
+      <c r="C95" s="11">
+        <v>1992</v>
+      </c>
+      <c r="D95" s="13">
+        <v>19786.400000000001</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1780,11 +1820,11 @@
       <c r="B96" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D96" s="8">
-        <v>91964.6</v>
+      <c r="C96" s="11">
+        <v>1993</v>
+      </c>
+      <c r="D96" s="13">
+        <v>235000</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -1794,11 +1834,11 @@
       <c r="B97" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D97" s="8">
-        <v>158015.59999999998</v>
+      <c r="C97" s="11">
+        <v>1994</v>
+      </c>
+      <c r="D97" s="13">
+        <v>23293.599999999999</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -1808,11 +1848,11 @@
       <c r="B98" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C98" s="7">
-        <v>2010</v>
-      </c>
-      <c r="D98" s="8">
-        <v>159048.6</v>
+      <c r="C98" s="11">
+        <v>1995</v>
+      </c>
+      <c r="D98" s="13">
+        <v>73862.399999999994</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -1822,11 +1862,11 @@
       <c r="B99" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="7">
-        <v>2011</v>
-      </c>
-      <c r="D99" s="8">
-        <v>39379.799999999996</v>
+      <c r="C99" s="11">
+        <v>1996</v>
+      </c>
+      <c r="D99" s="13">
+        <v>12893.8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -1836,11 +1876,11 @@
       <c r="B100" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C100" s="7">
-        <v>2012</v>
-      </c>
-      <c r="D100" s="8">
-        <v>163378.4</v>
+      <c r="C100" s="11">
+        <v>1997</v>
+      </c>
+      <c r="D100" s="13">
+        <v>40955.199999999997</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -1850,11 +1890,11 @@
       <c r="B101" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="7">
-        <v>2013</v>
-      </c>
-      <c r="D101" s="8">
-        <v>99140</v>
+      <c r="C101" s="11">
+        <v>1998</v>
+      </c>
+      <c r="D101" s="13">
+        <v>6140</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -1864,11 +1904,11 @@
       <c r="B102" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C102" s="7">
-        <v>2014</v>
-      </c>
-      <c r="D102" s="8">
-        <v>45921.599999999999</v>
+      <c r="C102" s="11">
+        <v>1999</v>
+      </c>
+      <c r="D102" s="13">
+        <v>9600</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -1878,11 +1918,11 @@
       <c r="B103" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="7">
-        <v>2015</v>
-      </c>
-      <c r="D103" s="8">
-        <v>158940.79999999999</v>
+      <c r="C103" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D103" s="13">
+        <v>37528</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -1892,11 +1932,11 @@
       <c r="B104" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C104" s="7">
-        <v>2016</v>
-      </c>
-      <c r="D104" s="8">
-        <v>212747.40000000002</v>
+      <c r="C104" s="11">
+        <v>2001</v>
+      </c>
+      <c r="D104" s="13">
+        <v>195124.6</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -1906,196 +1946,235 @@
       <c r="B105" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C105" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D105" s="8">
-        <v>0</v>
+      <c r="C105" s="11">
+        <v>2002</v>
+      </c>
+      <c r="D105" s="13">
+        <v>564876.80000000005</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C106" s="7">
-        <v>1912</v>
+      <c r="C106" s="11">
+        <v>2003</v>
+      </c>
+      <c r="D106" s="13">
+        <v>132728</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C107" s="7">
-        <v>1921</v>
+      <c r="C107" s="11">
+        <v>2004</v>
+      </c>
+      <c r="D107" s="13">
+        <v>20989</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="7">
-        <v>1938</v>
+      <c r="C108" s="11">
+        <v>2005</v>
+      </c>
+      <c r="D108" s="13">
+        <v>151697.79999999999</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="7">
-        <v>1941</v>
-      </c>
-      <c r="D109" s="6">
-        <v>200</v>
+      <c r="C109" s="11">
+        <v>2006</v>
+      </c>
+      <c r="D109" s="13">
+        <v>143002.59999999998</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="7">
-        <v>1950</v>
+      <c r="C110" s="11">
+        <v>2007</v>
+      </c>
+      <c r="D110" s="13">
+        <v>116791.59999999999</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C111" s="7">
-        <v>1952</v>
+      <c r="C111" s="11">
+        <v>2008</v>
+      </c>
+      <c r="D111" s="13">
+        <v>137691.40000000002</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C112" s="7">
-        <v>1955</v>
+      <c r="C112" s="11">
+        <v>2009</v>
+      </c>
+      <c r="D112" s="13">
+        <v>323274.80000000005</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C113" s="7">
-        <v>1956</v>
+      <c r="C113" s="11">
+        <v>2010</v>
+      </c>
+      <c r="D113" s="13">
+        <v>176390.2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="7">
-        <v>1962</v>
+      <c r="C114" s="11">
+        <v>2011</v>
+      </c>
+      <c r="D114" s="13">
+        <v>82089</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C115" s="7">
-        <v>1967</v>
+      <c r="C115" s="11">
+        <v>2012</v>
+      </c>
+      <c r="D115" s="13">
+        <v>216782</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C116" s="7">
-        <v>1970</v>
-      </c>
-      <c r="D116" s="6">
-        <v>16350</v>
+      <c r="C116" s="11">
+        <v>2013</v>
+      </c>
+      <c r="D116" s="13">
+        <v>214898</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C117" s="7">
-        <v>1972</v>
+      <c r="C117" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D117" s="13">
+        <v>63355.400000000009</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C118" s="7">
-        <v>1973</v>
+      <c r="C118" s="11">
+        <v>2015</v>
+      </c>
+      <c r="D118" s="13">
+        <v>270937.60000000003</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C119" s="7">
-        <v>1974</v>
+      <c r="C119" s="11">
+        <v>2016</v>
+      </c>
+      <c r="D119" s="13">
+        <v>529641.19999999995</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C120" s="7">
-        <v>1975</v>
-      </c>
-      <c r="D120" s="6">
-        <v>1569</v>
+      <c r="C120" s="11">
+        <v>2017</v>
+      </c>
+      <c r="D120" s="13">
+        <v>109469.4</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C121" s="7">
-        <v>1978</v>
+      <c r="C121" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D121" s="13">
+        <v>236334.4</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -2106,11 +2185,9 @@
         <v>12</v>
       </c>
       <c r="C122" s="7">
-        <v>1979</v>
-      </c>
-      <c r="D122" s="6">
-        <v>0</v>
-      </c>
+        <v>1912</v>
+      </c>
+      <c r="D122" s="9"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
@@ -2119,11 +2196,11 @@
       <c r="B123" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C123" s="7">
-        <v>1980</v>
-      </c>
-      <c r="D123" s="6">
-        <v>300</v>
+      <c r="C123" s="11">
+        <v>1916</v>
+      </c>
+      <c r="D123" s="13">
+        <v>5792</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -2133,9 +2210,10 @@
       <c r="B124" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C124" s="7">
-        <v>1981</v>
-      </c>
+      <c r="C124" s="11">
+        <v>1921</v>
+      </c>
+      <c r="D124" s="13"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
@@ -2144,12 +2222,10 @@
       <c r="B125" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C125" s="7">
-        <v>1982</v>
-      </c>
-      <c r="D125" s="6">
-        <v>550</v>
-      </c>
+      <c r="C125" s="11">
+        <v>1938</v>
+      </c>
+      <c r="D125" s="13"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
@@ -2158,8 +2234,11 @@
       <c r="B126" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="7">
-        <v>1983</v>
+      <c r="C126" s="11">
+        <v>1941</v>
+      </c>
+      <c r="D126" s="13">
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -2169,9 +2248,10 @@
       <c r="B127" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C127" s="7">
-        <v>1984</v>
-      </c>
+      <c r="C127" s="11">
+        <v>1946</v>
+      </c>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
@@ -2180,9 +2260,10 @@
       <c r="B128" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C128" s="7">
-        <v>1985</v>
-      </c>
+      <c r="C128" s="11">
+        <v>1950</v>
+      </c>
+      <c r="D128" s="13"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
@@ -2191,8 +2272,11 @@
       <c r="B129" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C129" s="7">
-        <v>1987</v>
+      <c r="C129" s="11">
+        <v>1952</v>
+      </c>
+      <c r="D129" s="13">
+        <v>800.6</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -2202,9 +2286,10 @@
       <c r="B130" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C130" s="7">
-        <v>1988</v>
-      </c>
+      <c r="C130" s="11">
+        <v>1955</v>
+      </c>
+      <c r="D130" s="13"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
@@ -2213,12 +2298,10 @@
       <c r="B131" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C131" s="7">
-        <v>1989</v>
-      </c>
-      <c r="D131" s="6">
-        <v>5150</v>
-      </c>
+      <c r="C131" s="11">
+        <v>1956</v>
+      </c>
+      <c r="D131" s="13"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
@@ -2227,9 +2310,10 @@
       <c r="B132" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C132" s="7">
-        <v>1990</v>
-      </c>
+      <c r="C132" s="11">
+        <v>1959</v>
+      </c>
+      <c r="D132" s="13"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
@@ -2238,8 +2322,11 @@
       <c r="B133" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C133" s="7">
-        <v>1991</v>
+      <c r="C133" s="11">
+        <v>1960</v>
+      </c>
+      <c r="D133" s="13">
+        <v>4530</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -2249,9 +2336,10 @@
       <c r="B134" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C134" s="7">
-        <v>1992</v>
-      </c>
+      <c r="C134" s="11">
+        <v>1962</v>
+      </c>
+      <c r="D134" s="13"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
@@ -2260,12 +2348,10 @@
       <c r="B135" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C135" s="7">
-        <v>1994</v>
-      </c>
-      <c r="D135" s="6">
-        <v>3505</v>
-      </c>
+      <c r="C135" s="11">
+        <v>1967</v>
+      </c>
+      <c r="D135" s="13"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
@@ -2274,11 +2360,11 @@
       <c r="B136" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C136" s="7">
-        <v>1995</v>
-      </c>
-      <c r="D136" s="6">
-        <v>2000</v>
+      <c r="C136" s="11">
+        <v>1970</v>
+      </c>
+      <c r="D136" s="13">
+        <v>16350</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -2288,11 +2374,11 @@
       <c r="B137" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C137" s="7">
-        <v>1996</v>
-      </c>
-      <c r="D137" s="6">
-        <v>20001</v>
+      <c r="C137" s="11">
+        <v>1972</v>
+      </c>
+      <c r="D137" s="13">
+        <v>110</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -2302,9 +2388,10 @@
       <c r="B138" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C138" s="7">
-        <v>1997</v>
-      </c>
+      <c r="C138" s="11">
+        <v>1973</v>
+      </c>
+      <c r="D138" s="13"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
@@ -2313,9 +2400,10 @@
       <c r="B139" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C139" s="7">
-        <v>1998</v>
-      </c>
+      <c r="C139" s="11">
+        <v>1974</v>
+      </c>
+      <c r="D139" s="13"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
@@ -2324,11 +2412,11 @@
       <c r="B140" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C140" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D140" s="6">
-        <v>36637</v>
+      <c r="C140" s="11">
+        <v>1975</v>
+      </c>
+      <c r="D140" s="13">
+        <v>1569</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -2338,11 +2426,11 @@
       <c r="B141" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C141" s="7">
-        <v>2001</v>
-      </c>
-      <c r="D141" s="6">
-        <v>5683.93</v>
+      <c r="C141" s="11">
+        <v>1976</v>
+      </c>
+      <c r="D141" s="13">
+        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -2352,8 +2440,11 @@
       <c r="B142" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C142" s="7">
-        <v>2002</v>
+      <c r="C142" s="11">
+        <v>1978</v>
+      </c>
+      <c r="D142" s="13">
+        <v>208</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -2363,12 +2454,10 @@
       <c r="B143" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C143" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D143" s="6">
-        <v>7539.16</v>
-      </c>
+      <c r="C143" s="11">
+        <v>1979</v>
+      </c>
+      <c r="D143" s="13"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
@@ -2377,8 +2466,11 @@
       <c r="B144" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C144" s="7">
-        <v>2004</v>
+      <c r="C144" s="11">
+        <v>1980</v>
+      </c>
+      <c r="D144" s="13">
+        <v>458</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -2388,12 +2480,10 @@
       <c r="B145" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C145" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D145" s="6">
-        <v>101875</v>
-      </c>
+      <c r="C145" s="11">
+        <v>1981</v>
+      </c>
+      <c r="D145" s="13"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
@@ -2402,11 +2492,11 @@
       <c r="B146" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C146" s="7">
-        <v>2006</v>
-      </c>
-      <c r="D146" s="6">
-        <v>12351.5</v>
+      <c r="C146" s="11">
+        <v>1982</v>
+      </c>
+      <c r="D146" s="13">
+        <v>550</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -2416,11 +2506,11 @@
       <c r="B147" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C147" s="7">
-        <v>2007</v>
-      </c>
-      <c r="D147" s="6">
-        <v>158933.84</v>
+      <c r="C147" s="11">
+        <v>1983</v>
+      </c>
+      <c r="D147" s="13">
+        <v>16217</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -2430,12 +2520,10 @@
       <c r="B148" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C148" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D148" s="6">
-        <v>29221.48</v>
-      </c>
+      <c r="C148" s="11">
+        <v>1984</v>
+      </c>
+      <c r="D148" s="13"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
@@ -2444,12 +2532,10 @@
       <c r="B149" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C149" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D149" s="6">
-        <v>67746.05</v>
-      </c>
+      <c r="C149" s="11">
+        <v>1985</v>
+      </c>
+      <c r="D149" s="13"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
@@ -2458,11 +2544,11 @@
       <c r="B150" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C150" s="7">
-        <v>2010</v>
-      </c>
-      <c r="D150" s="6">
-        <v>47179.3</v>
+      <c r="C150" s="11">
+        <v>1987</v>
+      </c>
+      <c r="D150" s="13">
+        <v>304</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -2472,12 +2558,10 @@
       <c r="B151" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C151" s="7">
-        <v>2011</v>
-      </c>
-      <c r="D151" s="6">
-        <v>72672.5</v>
-      </c>
+      <c r="C151" s="11">
+        <v>1988</v>
+      </c>
+      <c r="D151" s="13"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
@@ -2486,11 +2570,11 @@
       <c r="B152" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C152" s="7">
-        <v>2012</v>
-      </c>
-      <c r="D152" s="6">
-        <v>17871.120000000003</v>
+      <c r="C152" s="11">
+        <v>1989</v>
+      </c>
+      <c r="D152" s="13">
+        <v>5150</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -2500,11 +2584,11 @@
       <c r="B153" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C153" s="7">
-        <v>2013</v>
-      </c>
-      <c r="D153" s="6">
-        <v>28827</v>
+      <c r="C153" s="11">
+        <v>1990</v>
+      </c>
+      <c r="D153" s="13">
+        <v>7525</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -2514,12 +2598,10 @@
       <c r="B154" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C154" s="7">
-        <v>2014</v>
-      </c>
-      <c r="D154" s="6">
-        <v>33153.33</v>
-      </c>
+      <c r="C154" s="11">
+        <v>1991</v>
+      </c>
+      <c r="D154" s="13"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
@@ -2528,11 +2610,11 @@
       <c r="B155" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C155" s="7">
-        <v>2015</v>
-      </c>
-      <c r="D155" s="6">
-        <v>212291.28</v>
+      <c r="C155" s="11">
+        <v>1992</v>
+      </c>
+      <c r="D155" s="13">
+        <v>1151</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -2542,12 +2624,10 @@
       <c r="B156" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C156" s="7">
-        <v>2016</v>
-      </c>
-      <c r="D156" s="6">
-        <v>119859.76999999999</v>
-      </c>
+      <c r="C156" s="11">
+        <v>1993</v>
+      </c>
+      <c r="D156" s="13"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
@@ -2556,345 +2636,345 @@
       <c r="B157" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C157" s="7">
-        <v>2017</v>
-      </c>
-      <c r="D157" s="9"/>
+      <c r="C157" s="11">
+        <v>1994</v>
+      </c>
+      <c r="D157" s="13">
+        <v>3505</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C158" s="7">
-        <v>1912</v>
-      </c>
-      <c r="D158" s="6">
-        <v>53.137651821862342</v>
+      <c r="C158" s="11">
+        <v>1995</v>
+      </c>
+      <c r="D158" s="13">
+        <v>7600</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B159" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C159" s="7">
-        <v>1921</v>
-      </c>
-      <c r="D159" s="6">
-        <v>75</v>
+      <c r="C159" s="11">
+        <v>1996</v>
+      </c>
+      <c r="D159" s="13">
+        <v>20001</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B160" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C160" s="7">
-        <v>1938</v>
-      </c>
-      <c r="D160" s="6">
-        <v>1.214574898785425</v>
+      <c r="C160" s="11">
+        <v>1997</v>
+      </c>
+      <c r="D160" s="13">
+        <v>15000</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C161" s="7">
-        <v>1941</v>
-      </c>
-      <c r="D161" s="6">
-        <v>41.295546558704451</v>
+      <c r="C161" s="11">
+        <v>1998</v>
+      </c>
+      <c r="D161" s="13">
+        <v>350</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C162" s="7">
-        <v>1950</v>
-      </c>
-      <c r="D162" s="6">
-        <v>1039.55</v>
-      </c>
+      <c r="C162" s="11">
+        <v>1999</v>
+      </c>
+      <c r="D162" s="13"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B163" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C163" s="7">
-        <v>1952</v>
-      </c>
-      <c r="D163" s="6">
-        <v>31.578947368421051</v>
+      <c r="C163" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D163" s="13">
+        <v>36372</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C164" s="7">
-        <v>1955</v>
-      </c>
-      <c r="D164" s="6">
-        <v>470.85020242914976</v>
+      <c r="C164" s="11">
+        <v>2001</v>
+      </c>
+      <c r="D164" s="13">
+        <v>6067.45</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B165" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C165" s="7">
-        <v>1956</v>
-      </c>
-      <c r="D165" s="6">
-        <v>0</v>
+      <c r="C165" s="11">
+        <v>2002</v>
+      </c>
+      <c r="D165" s="13">
+        <v>106.57</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B166" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C166" s="7">
-        <v>1962</v>
-      </c>
-      <c r="D166" s="6">
-        <v>238.72874493927125</v>
+      <c r="C166" s="11">
+        <v>2003</v>
+      </c>
+      <c r="D166" s="13">
+        <v>7951.91</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B167" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C167" s="7">
-        <v>1967</v>
-      </c>
-      <c r="D167" s="6">
-        <v>0</v>
+      <c r="C167" s="11">
+        <v>2004</v>
+      </c>
+      <c r="D167" s="13">
+        <v>902.08</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B168" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C168" s="7">
-        <v>1970</v>
-      </c>
-      <c r="D168" s="6">
-        <v>17888.241902834008</v>
+      <c r="C168" s="11">
+        <v>2005</v>
+      </c>
+      <c r="D168" s="13">
+        <v>50875</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B169" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C169" s="7">
-        <v>1972</v>
-      </c>
-      <c r="D169" s="6">
-        <v>30</v>
+      <c r="C169" s="11">
+        <v>2006</v>
+      </c>
+      <c r="D169" s="13">
+        <v>52851.5</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C170" s="7">
-        <v>1973</v>
-      </c>
-      <c r="D170" s="6">
-        <v>42.510121457489873</v>
+      <c r="C170" s="11">
+        <v>2007</v>
+      </c>
+      <c r="D170" s="13">
+        <v>63410.840000000004</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C171" s="7">
-        <v>1974</v>
-      </c>
-      <c r="D171" s="6">
-        <v>36.032388663967609</v>
+      <c r="C171" s="11">
+        <v>2008</v>
+      </c>
+      <c r="D171" s="13">
+        <v>33039.25</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C172" s="7">
-        <v>1975</v>
-      </c>
-      <c r="D172" s="6">
-        <v>26610</v>
+      <c r="C172" s="11">
+        <v>2009</v>
+      </c>
+      <c r="D172" s="13">
+        <v>128302.2</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C173" s="7">
-        <v>1978</v>
-      </c>
-      <c r="D173" s="6">
-        <v>1000</v>
+      <c r="C173" s="11">
+        <v>2010</v>
+      </c>
+      <c r="D173" s="13">
+        <v>47251.369999999995</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B174" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C174" s="7">
-        <v>1979</v>
-      </c>
-      <c r="D174" s="6">
-        <v>37000</v>
+      <c r="C174" s="11">
+        <v>2011</v>
+      </c>
+      <c r="D174" s="13">
+        <v>77433.38</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C175" s="7">
-        <v>1980</v>
-      </c>
-      <c r="D175" s="6">
-        <v>1343.7246963562752</v>
+      <c r="C175" s="11">
+        <v>2012</v>
+      </c>
+      <c r="D175" s="13">
+        <v>22983.120000000003</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C176" s="7">
-        <v>1981</v>
-      </c>
-      <c r="D176" s="6">
-        <v>531.17408906882588</v>
+      <c r="C176" s="11">
+        <v>2013</v>
+      </c>
+      <c r="D176" s="13">
+        <v>82219.429999999993</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C177" s="7">
-        <v>1982</v>
-      </c>
-      <c r="D177" s="6">
-        <v>63003</v>
+      <c r="C177" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D177" s="13">
+        <v>33458.76</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C178" s="7">
-        <v>1983</v>
-      </c>
-      <c r="D178" s="6">
-        <v>80.97165991902834</v>
+      <c r="C178" s="11">
+        <v>2015</v>
+      </c>
+      <c r="D178" s="13">
+        <v>164525.50999999998</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C179" s="7">
-        <v>1984</v>
-      </c>
-      <c r="D179" s="6">
-        <v>26.315789473684209</v>
+      <c r="C179" s="11">
+        <v>2016</v>
+      </c>
+      <c r="D179" s="13">
+        <v>154601.27000000002</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C180" s="7">
-        <v>1985</v>
-      </c>
-      <c r="D180" s="6">
-        <v>0</v>
+      <c r="C180" s="11">
+        <v>2017</v>
+      </c>
+      <c r="D180" s="13">
+        <v>116134.76</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B181" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C181" s="7">
-        <v>1987</v>
-      </c>
-      <c r="D181" s="6">
-        <v>0</v>
+      <c r="C181" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D181" s="13">
+        <v>13342</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -2905,10 +2985,10 @@
         <v>12</v>
       </c>
       <c r="C182" s="7">
-        <v>1988</v>
-      </c>
-      <c r="D182" s="6">
-        <v>0</v>
+        <v>1912</v>
+      </c>
+      <c r="D182" s="10">
+        <v>53.15625</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -2918,11 +2998,11 @@
       <c r="B183" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C183" s="7">
-        <v>1989</v>
-      </c>
-      <c r="D183" s="6">
-        <v>5886.6396761133601</v>
+      <c r="C183" s="11">
+        <v>1916</v>
+      </c>
+      <c r="D183" s="14">
+        <v>800</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -2932,11 +3012,11 @@
       <c r="B184" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C184" s="7">
-        <v>1990</v>
-      </c>
-      <c r="D184" s="6">
-        <v>100.58704453441294</v>
+      <c r="C184" s="11">
+        <v>1921</v>
+      </c>
+      <c r="D184" s="14">
+        <v>75</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -2946,11 +3026,11 @@
       <c r="B185" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C185" s="7">
-        <v>1991</v>
-      </c>
-      <c r="D185" s="6">
-        <v>1500</v>
+      <c r="C185" s="11">
+        <v>1938</v>
+      </c>
+      <c r="D185" s="14">
+        <v>1.2150000000000001</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -2960,11 +3040,11 @@
       <c r="B186" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C186" s="7">
-        <v>1992</v>
-      </c>
-      <c r="D186" s="6">
-        <v>8505.2898785425095</v>
+      <c r="C186" s="11">
+        <v>1941</v>
+      </c>
+      <c r="D186" s="14">
+        <v>41.31</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -2974,11 +3054,11 @@
       <c r="B187" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C187" s="7">
-        <v>1994</v>
-      </c>
-      <c r="D187" s="6">
-        <v>2433.8582995951415</v>
+      <c r="C187" s="11">
+        <v>1946</v>
+      </c>
+      <c r="D187" s="14">
+        <v>1.12185</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
@@ -2988,11 +3068,11 @@
       <c r="B188" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C188" s="7">
-        <v>1995</v>
-      </c>
-      <c r="D188" s="6">
-        <v>3938.0566801619429</v>
+      <c r="C188" s="11">
+        <v>1950</v>
+      </c>
+      <c r="D188" s="14">
+        <v>1039.55</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
@@ -3002,11 +3082,11 @@
       <c r="B189" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C189" s="7">
-        <v>1996</v>
-      </c>
-      <c r="D189" s="6">
-        <v>1210.5263157894735</v>
+      <c r="C189" s="11">
+        <v>1952</v>
+      </c>
+      <c r="D189" s="14">
+        <v>30031.59</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -3016,11 +3096,11 @@
       <c r="B190" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C190" s="7">
-        <v>1997</v>
-      </c>
-      <c r="D190" s="6">
-        <v>10000</v>
+      <c r="C190" s="11">
+        <v>1955</v>
+      </c>
+      <c r="D190" s="14">
+        <v>471.01500000000004</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -3030,12 +3110,10 @@
       <c r="B191" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C191" s="7">
-        <v>1998</v>
-      </c>
-      <c r="D191" s="6">
-        <v>148.80000000000001</v>
-      </c>
+      <c r="C191" s="11">
+        <v>1956</v>
+      </c>
+      <c r="D191" s="14"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
@@ -3044,11 +3122,11 @@
       <c r="B192" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C192" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D192" s="6">
-        <v>3326.8421052631579</v>
+      <c r="C192" s="11">
+        <v>1959</v>
+      </c>
+      <c r="D192" s="14">
+        <v>1618</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
@@ -3058,11 +3136,11 @@
       <c r="B193" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C193" s="7">
-        <v>2001</v>
-      </c>
-      <c r="D193" s="6">
-        <v>7121.4574898785422</v>
+      <c r="C193" s="11">
+        <v>1960</v>
+      </c>
+      <c r="D193" s="14">
+        <v>35339.54</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
@@ -3072,11 +3150,11 @@
       <c r="B194" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C194" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D194" s="6">
-        <v>7400</v>
+      <c r="C194" s="11">
+        <v>1962</v>
+      </c>
+      <c r="D194" s="14">
+        <v>238.75</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
@@ -3086,12 +3164,10 @@
       <c r="B195" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C195" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D195" s="6">
-        <v>7270.2</v>
-      </c>
+      <c r="C195" s="11">
+        <v>1967</v>
+      </c>
+      <c r="D195" s="14"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
@@ -3100,11 +3176,11 @@
       <c r="B196" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C196" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D196" s="6">
-        <v>809.71659919028332</v>
+      <c r="C196" s="11">
+        <v>1970</v>
+      </c>
+      <c r="D196" s="14">
+        <v>17888.474999999999</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
@@ -3114,11 +3190,11 @@
       <c r="B197" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C197" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D197" s="6">
-        <v>12913.301619433198</v>
+      <c r="C197" s="11">
+        <v>1972</v>
+      </c>
+      <c r="D197" s="14">
+        <v>475.50000000000006</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
@@ -3128,11 +3204,11 @@
       <c r="B198" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C198" s="7">
-        <v>2006</v>
-      </c>
-      <c r="D198" s="6">
-        <v>12092.085910931175</v>
+      <c r="C198" s="11">
+        <v>1973</v>
+      </c>
+      <c r="D198" s="14">
+        <v>7542.5249999999996</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
@@ -3142,11 +3218,11 @@
       <c r="B199" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C199" s="7">
-        <v>2007</v>
-      </c>
-      <c r="D199" s="6">
-        <v>42603.604493927123</v>
+      <c r="C199" s="11">
+        <v>1974</v>
+      </c>
+      <c r="D199" s="14">
+        <v>36.045000000000002</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
@@ -3156,11 +3232,11 @@
       <c r="B200" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C200" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D200" s="6">
-        <v>11474.370971659919</v>
+      <c r="C200" s="11">
+        <v>1975</v>
+      </c>
+      <c r="D200" s="14">
+        <v>26610</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
@@ -3170,11 +3246,11 @@
       <c r="B201" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C201" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D201" s="6">
-        <v>19039.078947368416</v>
+      <c r="C201" s="11">
+        <v>1976</v>
+      </c>
+      <c r="D201" s="14">
+        <v>12362.625</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
@@ -3184,11 +3260,11 @@
       <c r="B202" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C202" s="7">
-        <v>2010</v>
-      </c>
-      <c r="D202" s="6">
-        <v>52996.719797570855</v>
+      <c r="C202" s="11">
+        <v>1978</v>
+      </c>
+      <c r="D202" s="14">
+        <v>14514.5</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
@@ -3198,11 +3274,11 @@
       <c r="B203" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C203" s="7">
-        <v>2011</v>
-      </c>
-      <c r="D203" s="6">
-        <v>202412.19817813765</v>
+      <c r="C203" s="11">
+        <v>1979</v>
+      </c>
+      <c r="D203" s="14">
+        <v>37000</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
@@ -3212,11 +3288,11 @@
       <c r="B204" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C204" s="7">
-        <v>2012</v>
-      </c>
-      <c r="D204" s="6">
-        <v>68810.765182186238</v>
+      <c r="C204" s="11">
+        <v>1980</v>
+      </c>
+      <c r="D204" s="14">
+        <v>4163.68</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
@@ -3226,11 +3302,11 @@
       <c r="B205" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C205" s="7">
-        <v>2013</v>
-      </c>
-      <c r="D205" s="6">
-        <v>19072.795425101212</v>
+      <c r="C205" s="11">
+        <v>1981</v>
+      </c>
+      <c r="D205" s="14">
+        <v>531.36</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
@@ -3240,11 +3316,11 @@
       <c r="B206" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C206" s="7">
-        <v>2014</v>
-      </c>
-      <c r="D206" s="6">
-        <v>21003.345101214567</v>
+      <c r="C206" s="11">
+        <v>1982</v>
+      </c>
+      <c r="D206" s="14">
+        <v>63003</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
@@ -3254,11 +3330,11 @@
       <c r="B207" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C207" s="7">
-        <v>2015</v>
-      </c>
-      <c r="D207" s="6">
-        <v>70287.061093117416</v>
+      <c r="C207" s="11">
+        <v>1983</v>
+      </c>
+      <c r="D207" s="14">
+        <v>22341.51</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
@@ -3268,11 +3344,11 @@
       <c r="B208" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C208" s="7">
-        <v>2016</v>
-      </c>
-      <c r="D208" s="6">
-        <v>49524.751295546557</v>
+      <c r="C208" s="11">
+        <v>1984</v>
+      </c>
+      <c r="D208" s="14">
+        <v>26.325000000000003</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
@@ -3282,11 +3358,457 @@
       <c r="B209" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C209" s="7">
+      <c r="C209" s="11">
+        <v>1985</v>
+      </c>
+      <c r="D209" s="14">
+        <v>21416.622750000002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C210" s="11">
+        <v>1987</v>
+      </c>
+      <c r="D210" s="14">
+        <v>909.87300000000016</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C211" s="11">
+        <v>1988</v>
+      </c>
+      <c r="D211" s="14"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C212" s="11">
+        <v>1989</v>
+      </c>
+      <c r="D212" s="14">
+        <v>5889</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C213" s="11">
+        <v>1990</v>
+      </c>
+      <c r="D213" s="14">
+        <v>100.62225000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C214" s="11">
+        <v>1991</v>
+      </c>
+      <c r="D214" s="14">
+        <v>1901.8639000000001</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C215" s="11">
+        <v>1992</v>
+      </c>
+      <c r="D215" s="14">
+        <v>9172.2800000000007</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C216" s="11">
+        <v>1993</v>
+      </c>
+      <c r="D216" s="14">
+        <v>350032</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C217" s="11">
+        <v>1994</v>
+      </c>
+      <c r="D217" s="14">
+        <v>2434.2901499999998</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C218" s="11">
+        <v>1995</v>
+      </c>
+      <c r="D218" s="14">
+        <v>5744.26</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C219" s="11">
+        <v>1996</v>
+      </c>
+      <c r="D219" s="14">
+        <v>1615.95</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220" s="11">
+        <v>1997</v>
+      </c>
+      <c r="D220" s="14">
+        <v>27187</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C221" s="11">
+        <v>1998</v>
+      </c>
+      <c r="D221" s="14">
+        <v>351.3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C222" s="11">
+        <v>1999</v>
+      </c>
+      <c r="D222" s="14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C223" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D223" s="14">
+        <v>22396.2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C224" s="11">
+        <v>2001</v>
+      </c>
+      <c r="D224" s="14">
+        <v>7415.7284500000005</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C225" s="11">
+        <v>2002</v>
+      </c>
+      <c r="D225" s="14">
+        <v>7017.8607000000002</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C226" s="11">
+        <v>2003</v>
+      </c>
+      <c r="D226" s="14">
+        <v>11286.389950000001</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C227" s="11">
+        <v>2004</v>
+      </c>
+      <c r="D227" s="14">
+        <v>32801.769</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C228" s="11">
+        <v>2005</v>
+      </c>
+      <c r="D228" s="14">
+        <v>19815.983949999998</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C229" s="11">
+        <v>2006</v>
+      </c>
+      <c r="D229" s="14">
+        <v>7201.2674999999999</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C230" s="11">
+        <v>2007</v>
+      </c>
+      <c r="D230" s="14">
+        <v>48161.002050000003</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C231" s="11">
+        <v>2008</v>
+      </c>
+      <c r="D231" s="14">
+        <v>90751.525599999994</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C232" s="11">
+        <v>2009</v>
+      </c>
+      <c r="D232" s="14">
+        <v>118996.75339999999</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C233" s="11">
+        <v>2010</v>
+      </c>
+      <c r="D233" s="14">
+        <v>53226.597099999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C234" s="11">
+        <v>2011</v>
+      </c>
+      <c r="D234" s="14">
+        <v>261115.83585</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C235" s="11">
+        <v>2012</v>
+      </c>
+      <c r="D235" s="14">
+        <v>83054.692999999999</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C236" s="11">
+        <v>2013</v>
+      </c>
+      <c r="D236" s="14">
+        <v>22434.14</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B237" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C237" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D237" s="14">
+        <v>30176.615750000004</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C238" s="11">
+        <v>2015</v>
+      </c>
+      <c r="D238" s="14">
+        <v>79976.656999999992</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C239" s="11">
+        <v>2016</v>
+      </c>
+      <c r="D239" s="14">
+        <v>219441.31069999994</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B240" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C240" s="11">
         <v>2017</v>
       </c>
-      <c r="D209" s="6">
-        <v>1008.0971659919028</v>
+      <c r="D240" s="14">
+        <v>33162.890849999996</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B241" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C241" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D241" s="14">
+        <v>2122.2081499999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>